<commit_message>
Lan Atazen Zerrenda bete
</commit_message>
<xml_diff>
--- a/Barne Informazioa/Barne Kudeaketa/Arrisku Zerrenda.xlsx
+++ b/Barne Informazioa/Barne Kudeaketa/Arrisku Zerrenda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Ingeniaritza Informatikoa\4. Maila\2. Lauhilekoa\GrAL\ProMeta\Barne Informazioa\Barne Kudeaketa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3021540-40E2-4B24-A556-BE7DCDE0DABA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060E7E7F-0004-4BBD-A23A-F2F8752D0E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Risks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Risks!$2:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Risks!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
     <author>mbarnard</author>
   </authors>
   <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Eranskin guztiak berrikusi, batez ere, proiektuaren hasieran idatzitakoak. Memoriak eranskinekiko lehentasuna duela zehaztu.</t>
-  </si>
-  <si>
-    <t>ProMeta: Arrisku Zerrenda</t>
   </si>
 </sst>
 </file>
@@ -199,7 +196,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -216,12 +213,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -243,12 +234,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -292,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -322,26 +319,25 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -747,10 +743,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="94" workbookViewId="0">
+      <selection sqref="A1:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -768,251 +764,263 @@
     <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="8" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>44252</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="7">
+        <f>+F2*G2</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>44252</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3" s="6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H3" s="7">
-        <f>+F3*G3</f>
-        <v>1</v>
+        <f t="shared" ref="H3:H19" si="0">+F3*G3</f>
+        <v>1.6</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>44252</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="6">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H4:H20" si="0">+F4*G4</f>
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>1.7999999999999998</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>44252</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="0"/>
-        <v>1.7999999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>44252</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="6">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="7">
         <f t="shared" si="0"/>
-        <v>3.2</v>
+        <v>1.5</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>44252</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7" s="6">
         <v>0.5</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5">
-        <v>44252</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1022,14 +1030,14 @@
     </row>
     <row r="10" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="10"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1039,14 +1047,14 @@
     </row>
     <row r="11" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1056,48 +1064,48 @@
     </row>
     <row r="12" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="2"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="13"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="10"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1107,14 +1115,14 @@
     </row>
     <row r="15" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1124,14 +1132,14 @@
     </row>
     <row r="16" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="9"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1141,7 +1149,7 @@
     </row>
     <row r="17" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="2"/>
@@ -1158,7 +1166,7 @@
     </row>
     <row r="18" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="2"/>
@@ -1175,37 +1183,20 @@
     </row>
     <row r="19" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="6"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>18</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Arriskuen zerrenda eta memoria arriskuen analisia
</commit_message>
<xml_diff>
--- a/Barne Informazioa/Barne Kudeaketa/Arrisku Zerrenda.xlsx
+++ b/Barne Informazioa/Barne Kudeaketa/Arrisku Zerrenda.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Ingeniaritza Informatikoa\4. Maila\2. Lauhilekoa\GrAL\ProMeta\Barne Informazioa\Barne Kudeaketa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julet\GitHub\ProMeta\Barne Informazioa\Barne Kudeaketa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060E7E7F-0004-4BBD-A23A-F2F8752D0E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9902A53D-756C-4B4D-8E8C-9028438D8450}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,24 +36,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>rbalduino</author>
     <author>mbarnard</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Type = I (indirect) or D (direct)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -111,9 +97,6 @@
     <t>Deskribapena</t>
   </si>
   <si>
-    <t>Mota</t>
-  </si>
-  <si>
     <t>Inpaktua</t>
   </si>
   <si>
@@ -123,21 +106,12 @@
     <t>Magnitudea</t>
   </si>
   <si>
-    <t>Jabea</t>
-  </si>
-  <si>
     <t>Mitigazio Estrategia</t>
   </si>
   <si>
     <t>Lan ingurunearen prestakuntza</t>
   </si>
   <si>
-    <t>Zuzena</t>
-  </si>
-  <si>
-    <t>JE</t>
-  </si>
-  <si>
     <t>Instalazioan zehar egindakoa dokumentu batean idatzi, instalatuko dudan softwarearen espezifikazioak ondo irakurri.</t>
   </si>
   <si>
@@ -187,6 +161,60 @@
   </si>
   <si>
     <t>Eranskin guztiak berrikusi, batez ere, proiektuaren hasieran idatzitakoak. Memoriak eranskinekiko lehentasuna duela zehaztu.</t>
+  </si>
+  <si>
+    <t>Memoria idazteko denbora falta</t>
+  </si>
+  <si>
+    <t>Memoria osoa ez utzi bukerarako, pixkanaka kapitulu batzuk idazten joan nahiz eta proiektua bukatu gabe egon.</t>
+  </si>
+  <si>
+    <t>Gerta daiteke memoria idazteko denbora nahikoa ez izatea, bukaerarako uzten bada. Oso garrantzitsua da momoria ondo idaztea.</t>
+  </si>
+  <si>
+    <t>Proiektua amaitzeko denbora falta</t>
+  </si>
+  <si>
+    <t>Baliteke proiektua amaitzeko denboraz juxtu ibiltzea. Horrek kalitatea jaistea eragin dezake, lana presaka egiteagatik.</t>
+  </si>
+  <si>
+    <t>Lana modu egokian antolatu eta konstantea izaten saiatu. Denbora aprobetxatu eta gauza garrantzitsuenetan zentratu. Ez dago dena bukatu beharrik, etorkizuneko lan bezala utz daiteke.</t>
+  </si>
+  <si>
+    <t>Egindako lanaren galera</t>
+  </si>
+  <si>
+    <t>Egindako lana galtzeak lana berregin behar izatea eragin dezake. Honek denbora galtzeaz gain frustrazioa eragiten du.</t>
+  </si>
+  <si>
+    <t>Bertsio kontrola erabili proiektuaren informazio guztia gordetzeko. Datu guztien segurtasun kopiak egin egunero.</t>
+  </si>
+  <si>
+    <t>Ordenagailuarekin arazoak</t>
+  </si>
+  <si>
+    <t>Nire ordenagailuarekin arazoak izateak denbora galtzeak eragin ditzake. Ordenagailua konpondu bitartean lana egin ahal ez izatea eragin dezake.</t>
+  </si>
+  <si>
+    <t>Makina birtualarekin arazoak</t>
+  </si>
+  <si>
+    <t>Alternatiba moduan lanerako tutoreak emandako makina birtuala edukitzea.</t>
+  </si>
+  <si>
+    <t>Makina birtualekin arazoak izateak lanerako ingurune hori eskuragarri ez izatea eragin dezake. Nire kasuan ordenagailu pertsonala erabili dudanez ez dauka eragin handirik.</t>
+  </si>
+  <si>
+    <t>Ordenagailu pertsonala erabili garapenerako ingurune nagusi moduan. Makina birtuala alternatiba moduan eduki arazoren bat badago erabiltzeko.</t>
+  </si>
+  <si>
+    <t>Proiektuaren planteamendu aldaketa</t>
+  </si>
+  <si>
+    <t>Proiektuan ziurgabetasun handia dagoenez, hurbilpen aldaketak egon daitezke. Honek atzerapenak eragin ditzake.</t>
+  </si>
+  <si>
+    <t>Proiektuaren osagaiak ahalik eta flexibleenak egiten saiatu. Horrela, hurbilpena aldatu arren egindako lana aprobetxatu daiteke.</t>
   </si>
 </sst>
 </file>
@@ -196,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -226,12 +254,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -289,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -329,9 +351,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -743,10 +762,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="94" workbookViewId="0">
-      <selection sqref="A1:J19"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -755,48 +774,40 @@
     <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="35.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="3.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -804,32 +815,26 @@
         <v>44252</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="2">
         <v>2</v>
       </c>
-      <c r="G2" s="6">
+      <c r="F2" s="6">
         <v>0.5</v>
       </c>
-      <c r="H2" s="7">
-        <f>+F2*G2</f>
+      <c r="G2" s="7">
+        <f>+E2*F2</f>
         <v>1</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -837,32 +842,26 @@
         <v>44252</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
         <v>4</v>
       </c>
-      <c r="G3" s="6">
+      <c r="F3" s="6">
         <v>0.4</v>
       </c>
-      <c r="H3" s="7">
-        <f t="shared" ref="H3:H19" si="0">+F3*G3</f>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G13" si="0">+E3*F3</f>
         <v>1.6</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -870,32 +869,26 @@
         <v>44252</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2">
         <v>3</v>
       </c>
-      <c r="G4" s="6">
+      <c r="F4" s="6">
         <v>0.6</v>
       </c>
-      <c r="H4" s="7">
+      <c r="G4" s="7">
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -903,32 +896,26 @@
         <v>44252</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" s="6">
+      <c r="F5" s="6">
         <v>0.8</v>
       </c>
-      <c r="H5" s="7">
+      <c r="G5" s="7">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="H5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -936,32 +923,26 @@
         <v>44252</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="6">
+      <c r="F6" s="6">
         <v>0.5</v>
       </c>
-      <c r="H6" s="7">
+      <c r="G6" s="7">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -969,234 +950,186 @@
         <v>44252</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="6">
+      <c r="F7" s="6">
         <v>0.5</v>
       </c>
-      <c r="H7" s="7">
+      <c r="G7" s="7">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7">
+      <c r="B8" s="5">
+        <v>44341</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7">
+      <c r="B9" s="5">
+        <v>44341</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7">
+      <c r="B10" s="5">
+        <v>44341</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="7">
+      <c r="B11" s="5">
+        <v>44341</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="7">
+      <c r="B12" s="12">
+        <v>44341</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="13">
+        <v>2</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="7">
+      <c r="B13" s="5">
+        <v>44341</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>